<commit_message>
damage on successful save
</commit_message>
<xml_diff>
--- a/data/sample/character_info.xlsx
+++ b/data/sample/character_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei\Documents\studies\programming\github\monte_carlo\data\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA82903F-50D7-4092-AE21-2283E71A43C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAF54F5-C4A1-4803-8082-CC374F591B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2466BF5D-C1D0-43BC-82BA-7C4FF8E9AFCE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2466BF5D-C1D0-43BC-82BA-7C4FF8E9AFCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Heroes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Type</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>1d8+2</t>
+  </si>
+  <si>
+    <t>saved_damage</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC8D62B-B5D1-4A4E-99B1-2859F2EF776B}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +514,7 @@
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,10 +570,13 @@
         <v>20</v>
       </c>
       <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -613,11 +619,11 @@
       <c r="O2">
         <v>2</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -660,11 +666,11 @@
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -713,7 +719,10 @@
       <c r="R4" t="s">
         <v>26</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4">
+        <v>0.5</v>
+      </c>
+      <c r="T4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -725,10 +734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAF54F7-3A13-4E71-A750-9DB0C83FC03E}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +745,7 @@
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -792,10 +801,13 @@
         <v>20</v>
       </c>
       <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -838,11 +850,11 @@
       <c r="O2">
         <v>2</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -885,11 +897,11 @@
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -938,7 +950,10 @@
       <c r="R4" t="s">
         <v>26</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Damage can now include several dice, e.g. 1d6+2d4+3
</commit_message>
<xml_diff>
--- a/data/sample/character_info.xlsx
+++ b/data/sample/character_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei\Documents\studies\programming\github\monte_carlo\data\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAF54F5-C4A1-4803-8082-CC374F591B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A288862-82A2-4BC8-8C5C-8F61727719AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2466BF5D-C1D0-43BC-82BA-7C4FF8E9AFCE}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>Fighter</t>
   </si>
   <si>
-    <t>1d12+4</t>
-  </si>
-  <si>
     <t>Cleric</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>saved_damage</t>
+  </si>
+  <si>
+    <t>1d12+1d6+4</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T4"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,7 +570,7 @@
         <v>20</v>
       </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T1" t="s">
         <v>17</v>
@@ -667,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -708,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4">
         <v>2</v>
@@ -717,13 +717,13 @@
         <v>13</v>
       </c>
       <c r="R4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S4">
         <v>0.5</v>
       </c>
       <c r="T4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +737,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +801,7 @@
         <v>20</v>
       </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T1" t="s">
         <v>17</v>
@@ -812,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -898,7 +898,7 @@
         <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -906,7 +906,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4">
         <v>2</v>
@@ -948,13 +948,13 @@
         <v>13</v>
       </c>
       <c r="R4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
         <v>26</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding data dictionary to sample file
</commit_message>
<xml_diff>
--- a/data/sample/character_info.xlsx
+++ b/data/sample/character_info.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei\Documents\studies\programming\github\monte_carlo\data\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A288862-82A2-4BC8-8C5C-8F61727719AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CE432A-60FA-411E-A781-95D19FED7D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2466BF5D-C1D0-43BC-82BA-7C4FF8E9AFCE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2466BF5D-C1D0-43BC-82BA-7C4FF8E9AFCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Heroes" sheetId="1" r:id="rId1"/>
     <sheet name="Monsters" sheetId="2" r:id="rId2"/>
+    <sheet name="Column dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
   <si>
     <t>Type</t>
   </si>
@@ -139,6 +140,96 @@
   </si>
   <si>
     <t>1d12+1d6+4</t>
+  </si>
+  <si>
+    <t>Column name</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Type of creature. Currently two types of characters are supported: Martials (e.g. Fighter) and Blasters (e.g. throw a fireball)</t>
+  </si>
+  <si>
+    <t>Name of creature.</t>
+  </si>
+  <si>
+    <t>Creature's AC</t>
+  </si>
+  <si>
+    <t>Bonus to save</t>
+  </si>
+  <si>
+    <t>Bonus to initiative</t>
+  </si>
+  <si>
+    <t>Bonus to attack</t>
+  </si>
+  <si>
+    <t>Can this character heal? Takes values of True or False.</t>
+  </si>
+  <si>
+    <t>Healing amount, only relevant if the character can heal. If healer=True but amount is missing, error is raised.</t>
+  </si>
+  <si>
+    <t>Required?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health of creature. All creatures are assumed to start at max health. </t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>True/False</t>
+  </si>
+  <si>
+    <t>Martial/Blaster</t>
+  </si>
+  <si>
+    <t>e.g. 1d4+4</t>
+  </si>
+  <si>
+    <t>str/dex/con/wis/cha/int</t>
+  </si>
+  <si>
+    <t>Martial only</t>
+  </si>
+  <si>
+    <t>Blaster only</t>
+  </si>
+  <si>
+    <t>Number of targets Blaster's spell attacks on average.</t>
+  </si>
+  <si>
+    <t>Number of attacks Martial creature can make.</t>
+  </si>
+  <si>
+    <t>Spell save DC (Blaster)</t>
+  </si>
+  <si>
+    <t>Save that targets need to make against Blaster's spell (e.g. dex for fireball)</t>
+  </si>
+  <si>
+    <t>Damage target takes if it succeeds the saving throw: 0 for no damage, 0.5 for half-damage</t>
+  </si>
+  <si>
+    <t>Damage of attack/spell</t>
+  </si>
+  <si>
+    <t>e.g. 2d6+1d4+4</t>
   </si>
 </sst>
 </file>
@@ -498,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC8D62B-B5D1-4A4E-99B1-2859F2EF776B}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAF54F7-3A13-4E71-A750-9DB0C83FC03E}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -961,4 +1052,320 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A775AE8C-83F4-4C7F-85B8-1A0CC2C8FE4F}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>